<commit_message>
Kruskal-Wallis, Dunn's test update
</commit_message>
<xml_diff>
--- a/Figure3/Fig3 data.xlsx
+++ b/Figure3/Fig3 data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcsegura/Desktop/PP4_github/Figure3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103EE4CC-2A34-8E4B-9D67-27A594249AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C020C725-8722-D848-AA1D-D2DAE5133706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23740" yWindow="3680" windowWidth="20540" windowHeight="15380" xr2:uid="{A544D509-C476-1649-B94C-AC6AAF619ED9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{A544D509-C476-1649-B94C-AC6AAF619ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 3D, E, F, I, J, K " sheetId="1" r:id="rId1"/>
     <sheet name="STATS" sheetId="6" r:id="rId2"/>
+    <sheet name="KW-test" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="68">
   <si>
     <t>file name</t>
   </si>
@@ -230,13 +231,33 @@
   <si>
     <t>3K</t>
   </si>
+  <si>
+    <t>H-statistic</t>
+  </si>
+  <si>
+    <t>Kruskal-Willis Test</t>
+  </si>
+  <si>
+    <t>Dunn's Comparison Test</t>
+  </si>
+  <si>
+    <t>Dunn's Test (No Correction)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -264,9 +285,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C26C335-6311-A644-AFCE-D97FE2889C11}">
   <dimension ref="A1:P158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
@@ -7491,4 +7515,538 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7991A9B-27B5-B543-A285-69B14BA57713}">
+  <dimension ref="A1:R14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>28.0379492600422</v>
+      </c>
+      <c r="F3" s="1">
+        <v>8.1589951738754896E-7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>30.150932911730798</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.8366653651354499E-7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>23.724418604651099</v>
+      </c>
+      <c r="F5" s="1">
+        <v>7.0519294176120597E-6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" t="s">
+        <v>42</v>
+      </c>
+      <c r="M8" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>47</v>
+      </c>
+      <c r="R8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>20</v>
+      </c>
+      <c r="J9">
+        <v>3.3469642214122</v>
+      </c>
+      <c r="K9">
+        <v>2.8909010587786201</v>
+      </c>
+      <c r="L9">
+        <v>0.76415747548728596</v>
+      </c>
+      <c r="M9">
+        <v>0.55770351725329204</v>
+      </c>
+      <c r="N9" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" t="s">
+        <v>50</v>
+      </c>
+      <c r="P9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>8.62039E-2</v>
+      </c>
+      <c r="R9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>13</v>
+      </c>
+      <c r="J10">
+        <v>3.3469642214122</v>
+      </c>
+      <c r="K10">
+        <v>1.3240875852182099</v>
+      </c>
+      <c r="L10">
+        <v>0.76415747548728596</v>
+      </c>
+      <c r="M10">
+        <v>0.28862825242440598</v>
+      </c>
+      <c r="N10" t="s">
+        <v>50</v>
+      </c>
+      <c r="O10" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>5.5509600000000001E-5</v>
+      </c>
+      <c r="R10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>20</v>
+      </c>
+      <c r="J11">
+        <v>1.29981904185996</v>
+      </c>
+      <c r="K11">
+        <v>2.7630235232906899</v>
+      </c>
+      <c r="L11">
+        <v>0.36483536618364298</v>
+      </c>
+      <c r="M11">
+        <v>0.63230008370938495</v>
+      </c>
+      <c r="N11" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11" t="s">
+        <v>50</v>
+      </c>
+      <c r="P11" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>2.4010299999999999E-5</v>
+      </c>
+      <c r="R11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>13</v>
+      </c>
+      <c r="J12">
+        <v>1.29981904185996</v>
+      </c>
+      <c r="K12">
+        <v>1.1592592947581799</v>
+      </c>
+      <c r="L12">
+        <v>0.36483536618364298</v>
+      </c>
+      <c r="M12">
+        <v>0.31828022894332803</v>
+      </c>
+      <c r="N12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P12" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0.29055300000000001</v>
+      </c>
+      <c r="R12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>20</v>
+      </c>
+      <c r="J13">
+        <v>2.6349345801108601</v>
+      </c>
+      <c r="K13">
+        <v>1.0797284114215699</v>
+      </c>
+      <c r="L13">
+        <v>0.48468467378554803</v>
+      </c>
+      <c r="M13">
+        <v>0.25510289935962399</v>
+      </c>
+      <c r="N13" t="s">
+        <v>50</v>
+      </c>
+      <c r="O13" t="s">
+        <v>50</v>
+      </c>
+      <c r="P13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>1.0854400000000001E-5</v>
+      </c>
+      <c r="R13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="J14">
+        <v>2.6349345801108601</v>
+      </c>
+      <c r="K14">
+        <v>1.18173099828129</v>
+      </c>
+      <c r="L14">
+        <v>0.48468467378554803</v>
+      </c>
+      <c r="M14">
+        <v>0.285971215631941</v>
+      </c>
+      <c r="N14" t="s">
+        <v>50</v>
+      </c>
+      <c r="O14" t="s">
+        <v>50</v>
+      </c>
+      <c r="P14" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>5.5509600000000001E-5</v>
+      </c>
+      <c r="R14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A7:R7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>